<commit_message>
all imgs converted to webp format
</commit_message>
<xml_diff>
--- a/react-vn-website/public/data/events.xlsx
+++ b/react-vn-website/public/data/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshi\Desktop\VN-Website\react-vn-website\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshi\Desktop\Vishwa Netrutvam\react-vn-website\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0741F88C-3A44-41FE-9313-C9DFFE5FF028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F0835A-D665-48C6-B035-6809D4F6CF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0E7DEA41-EDEA-4EC2-A269-A03937E96D1B}"/>
+    <workbookView xWindow="9060" yWindow="612" windowWidth="10140" windowHeight="10572" firstSheet="2" activeTab="3" xr2:uid="{0E7DEA41-EDEA-4EC2-A269-A03937E96D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="2021-22" sheetId="4" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>https://drive.google.com/file/d/1wo8kvsMQUm5Jx1HDTcEvBXRO1GJv9ser/view?usp=drive_link</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1YdWD8Q_O_Ml_2X7vdiIBvUPnGUQzF1HI/view?usp=drive_link</t>
-  </si>
-  <si>
     <t>SYDA Student Induction Program</t>
   </si>
   <si>
@@ -202,39 +199,6 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1v4MkOTMg_IJwx9Q1cwQJGfGWat05MNlU/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E1/image1.JPG, /images/Events/2024-25/E1/image2.JPG, /images/Events/2024-25/E1/image3.JPG</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E2/image1.jpg, /images/Events/2024-25/E2/image2.jpg, /images/Events/2024-25/E2/image3.jpg</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E3/image1.jpg, /images/Events/2024-25/E3/image2.jpg, /images/Events/2024-25/E3/image3.jpg, /images/Events/2024-25/E3/image4.jpg</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E4/image1.jpg, /images/Events/2024-25/E4/image2.jpg, /images/Events/2024-25/E4/image3.jpg, /images/Events/2024-25/E4/image4.jpg</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E5/image1.jpg, /images/Events/2024-25/E5/image2.JPG, /images/Events/2024-25/E5/image3.JPG, /images/Events/2024-25/E5/image4.jpg</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E7/image1.jpg, /images/Events/2024-25/E7/image2.PNG</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E8/image1.jpg, /images/Events/2024-25/E8/image2.jpg, /images/Events/2024-25/E8/image3.jpeg, /images/Events/2024-25/E8/image4.jpg, /images/Events/2024-25/E8/image5.JPG</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E11/img1.JPG, /images/Events/2024-25/E11/img2.JPG, /images/Events/2024-25/E11/img3.JPG, /images/Events/2024-25/E11/img4.JPG,/images/Events/2024-25/E11/img5.JPG</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E9/image1.jpg, /images/Events/2024-25/E9/image2.jpg, /images/Events/2024-25/E9/image3.jpg, /images/Events/2024-25/E9/image4.jpg</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E10/1.jpg, /images/Events/2024-25/E10/2.JPG, /images/Events/2024-25/E10/3.JPG, /images/Events/2024-25/E10/4.jpg,/images/Events/2024-25/E10/5.JPG</t>
-  </si>
-  <si>
-    <t>/images/Events/2024-25/E6/image1.png, /images/Events/2024-25/E6/image2.png, /images/Events/2024-25/E6/image3.png, /images/Events/2024-25/E6/image4.png</t>
   </si>
   <si>
     <t>In September 2024, Vishwa Netrutvam welcomed the incoming batch to VIT Pune at the First Year Induction program held in Sharad Arena. Online induction sessions were conducted in multiple slots, familiarizing students with our initiatives. The event marked the beginning of an exciting journey for the new batch with Team Vishwa Netrutvam!</t>
@@ -318,6 +282,42 @@
   </si>
   <si>
     <t>Six Sigma Workshop by Mr. Subhash Aaghashe</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E2/image1.webp, /images/Events/2024-25/E2/image2.webp, /images/Events/2024-25/E2/image3.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E3/image1.webp, /images/Events/2024-25/E3/image2.webp, /images/Events/2024-25/E3/image3.webp, /images/Events/2024-25/E3/image4.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E4/image1.webp, /images/Events/2024-25/E4/image2.webp, /images/Events/2024-25/E4/image3.webp, /images/Events/2024-25/E4/image4.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E5/image1.webp, /images/Events/2024-25/E5/image2.webp, /images/Events/2024-25/E5/image3.webp, /images/Events/2024-25/E5/image4.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E9/image1.webp, /images/Events/2024-25/E9/image2.webp, /images/Events/2024-25/E9/image3.webp, /images/Events/2024-25/E9/image4.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E10/1.webp, /images/Events/2024-25/E10/2.webp, /images/Events/2024-25/E10/3.webp, /images/Events/2024-25/E10/4.webp,/images/Events/2024-25/E10/5.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E11/img1.webp, /images/Events/2024-25/E11/img2.webp, /images/Events/2024-25/E11/img3.webp, /images/Events/2024-25/E11/img4.webp,/images/Events/2024-25/E11/img5.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E1/image1.webp, /images/Events/2024-25/E1/image2.webp, /images/Events/2024-25/E1/image3.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E7/image1.webp, /images/Events/2024-25/E7/image2.webp</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1YdWD8Q_O_Ml_2X7vdiIBvUwebpUQzF1HI/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E6/image1.webp, /images/Events/2024-25/E6/image2.webp, /images/Events/2024-25/E6/image3.webp, /images/Events/2024-25/E6/image4.webp</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E8/image1.webp, /images/Events/2024-25/E8/image2.webp, /images/Events/2024-25/E8/image3.webp, /images/Events/2024-25/E8/image4.webp, /images/Events/2024-25/E8/image5.webp</t>
   </si>
 </sst>
 </file>
@@ -742,7 +742,7 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4">
         <v>44618</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B5" s="6">
         <v>44625</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4">
         <v>44646</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4">
         <v>44688</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B2" s="4">
         <v>44819</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B6" s="5">
         <v>45008</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B8" s="4">
         <v>45037</v>
@@ -931,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201B4819-9FEA-4AA1-A31F-6B3F9660C60D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -957,7 +957,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B2" s="6">
         <v>45200</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="3" spans="1:4" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7">
         <v>45303</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B4" s="4">
         <v>45336</v>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC42FBBC-526B-47C1-AEBC-8D264F65DB64}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,13 +1055,13 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1073,13 +1073,13 @@
         <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1091,13 +1091,13 @@
         <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -1109,13 +1109,13 @@
         <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -1127,47 +1127,47 @@
         <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6">
         <v>45560</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -1176,16 +1176,16 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1194,16 +1194,16 @@
         <v>45575</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -1212,16 +1212,16 @@
         <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -1230,10 +1230,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -1285,8 +1285,9 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{EA96B73E-A63A-4663-8EA0-EF1D1C0FFB82}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{1DC8C946-6743-4347-A456-7265E8911A71}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{D21018FF-1549-4F52-8372-81E669F741D2}"/>
-    <hyperlink ref="D9" r:id="rId6" xr:uid="{34CEDF06-3CE7-4D94-AAC0-912C3FB437D0}"/>
+    <hyperlink ref="D9" r:id="rId6" display="https://drive.google.com/file/d/1YdWD8Q_O_Ml_2X7vdiIBvUPnGUQzF1HI/view?usp=drive_link" xr:uid="{34CEDF06-3CE7-4D94-AAC0-912C3FB437D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
required changes almost done
</commit_message>
<xml_diff>
--- a/react-vn-website/public/data/events.xlsx
+++ b/react-vn-website/public/data/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshi\Desktop\Vishwa Netrutvam\react-vn-website\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75975C3-F384-40B5-87FA-2F050122F359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F2651-4969-45E1-9F2D-F922BED4A2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6972" yWindow="0" windowWidth="14532" windowHeight="12240" firstSheet="2" activeTab="3" xr2:uid="{0E7DEA41-EDEA-4EC2-A269-A03937E96D1B}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="3" xr2:uid="{0E7DEA41-EDEA-4EC2-A269-A03937E96D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="2021-22" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="143">
   <si>
     <t>link</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1VaDpKWTx6nbMmy-PgdW-A0gXv_S5zx_e/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1Ox-gYnuOJNqjNCDImVbe8HOuJLVq9tW5/view?usp=drive_link</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1wo8kvsMQUm5Jx1HDTcEvBXRO1GJv9ser/view?usp=drive_link</t>
@@ -446,15 +443,9 @@
     <t>/images/Events/2024-25/E18/img1.webp, /images/Events/2024-25/E18/img2.webp, /images/Events/2024-25/E18/img3.webp, /images/Events/2024-25/E18/img4.webp,/images/Events/2024-25/E18/img5.webp,/images/Events/2024-25/E18/img6.webp</t>
   </si>
   <si>
-    <t>March 26, 2025</t>
-  </si>
-  <si>
     <t>February 20, 2025</t>
   </si>
   <si>
-    <t>Expert Lecture Series with Regal Rexnord Corporation on 'System Design (Conveying)' by Mr. Swapnil Raut &amp; Mr. Chaitanya Raut</t>
-  </si>
-  <si>
     <t>On 2nd April 2025, we hosted an Expert Lecture Series on 'Gearbox Design Basics' with industry experts Mr. Sachin Jagadale and Mr. Shivakumar Choughule from Regal Rexnord Corporation. The session covered gearbox mechanisms, design parameters, and industry applications, providing students with practical insights into mechanical design challenges and solutions.</t>
   </si>
   <si>
@@ -480,6 +471,30 @@
   </si>
   <si>
     <t>/images/Events/2024-25/E21/img1.webp,/images/Events/2024-25/E21/img2.webp, /images/Events/2024-25/E21/img3.webp,/images/Events/2024-25/E21/img4.webp,/images/Events/2024-25/E21/img5.webp</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1pzRmzeElL3uQVhkLbBq4WFClxAibKjAl/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>March 27, 2025</t>
+  </si>
+  <si>
+    <t>April 9, 2025</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1Qqo_RpDIIN3bhNVOkHrpGebD-TUrNLxa?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Expert Lecture on 'A Complete Guide To Build Your Startups' by Mr. Akash Deshpande, Co-Founder &amp; CTO, Gaana AI</t>
+  </si>
+  <si>
+    <t>On 10th April 2025, Vishwa Netrutvam &amp; Office of Student Counselling &amp; Career Guidance jointly hosted an expert lecture on "A Complete Guide To Build Your Startups" by Mr. Akash Deshpande, Co-Founder &amp; CTO, Gaana AI. The session provided a comprehensive guide to building successful startups, covering key aspects and strategies for entrepreneurs.</t>
+  </si>
+  <si>
+    <t>/images/Events/2024-25/E22/img1.webp,/images/Events/2024-25/E22/img2.webp, /images/Events/2024-25/E22/img3.webp,/images/Events/2024-25/E22/img4.webp</t>
+  </si>
+  <si>
+    <t>Expert Lecture Series with Regal Rexnord Corporation on 'System Design (Conveying)' by Mr. Swapnil Raut &amp; Mr. Chaitanya Kulkarni</t>
   </si>
 </sst>
 </file>
@@ -935,7 +950,7 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -943,7 +958,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4">
         <v>44618</v>
@@ -951,7 +966,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="6">
         <v>44625</v>
@@ -959,7 +974,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -967,7 +982,7 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="4">
         <v>44646</v>
@@ -975,7 +990,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="4">
         <v>44688</v>
@@ -1019,7 +1034,7 @@
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4">
         <v>44819</v>
@@ -1063,7 +1078,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="5">
         <v>45008</v>
@@ -1085,7 +1100,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="4">
         <v>45037</v>
@@ -1150,7 +1165,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="6">
         <v>45200</v>
@@ -1158,7 +1173,7 @@
     </row>
     <row r="3" spans="1:4" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7">
         <v>45303</v>
@@ -1170,7 +1185,7 @@
     </row>
     <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4">
         <v>45336</v>
@@ -1202,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC42FBBC-526B-47C1-AEBC-8D264F65DB64}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,13 +1264,13 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1267,13 +1282,13 @@
         <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1285,13 +1300,13 @@
         <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -1300,16 +1315,16 @@
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -1318,50 +1333,50 @@
         <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="13">
         <v>45560</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -1370,16 +1385,16 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1388,16 +1403,16 @@
         <v>45575</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -1406,16 +1421,16 @@
         <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -1424,186 +1439,203 @@
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>137</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1624,8 +1656,9 @@
     <hyperlink ref="D20" r:id="rId14" xr:uid="{CAAC99B1-CB6E-429C-A20C-A7C12C258A71}"/>
     <hyperlink ref="D21" r:id="rId15" xr:uid="{2E402B33-27B0-431D-B6AA-AAAD83799686}"/>
     <hyperlink ref="D22" r:id="rId16" xr:uid="{6D5CAA12-324B-4329-AB7A-679B9B900D75}"/>
+    <hyperlink ref="D23" r:id="rId17" xr:uid="{4CB93F28-C571-46D9-9F98-66F941ED8FA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>